<commit_message>
ui fixes and changes in offer workbook
</commit_message>
<xml_diff>
--- a/api/resources/excel/offer_workbook/offer_workbook.xlsx
+++ b/api/resources/excel/offer_workbook/offer_workbook.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
   <si>
     <t>offer_table</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t>public</t>
+  </si>
+  <si>
+    <t>coupon_id</t>
+  </si>
+  <si>
+    <t>campaign_id</t>
   </si>
 </sst>
 </file>
@@ -603,6 +609,40 @@
         <v>35</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>

</xml_diff>

<commit_message>
modified: offer view, offer workbook and apis related to offers and redeemCouponCode
</commit_message>
<xml_diff>
--- a/api/resources/excel/offer_workbook/offer_workbook.xlsx
+++ b/api/resources/excel/offer_workbook/offer_workbook.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
   <si>
     <t>offer_table</t>
   </si>
@@ -85,10 +85,13 @@
     <t>number</t>
   </si>
   <si>
+    <t>discount_upto</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>item_constraint</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>all, specific</t>
@@ -544,27 +547,27 @@
         <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="K8" s="1">
+        <v>100.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="1">
-        <v>50.0</v>
+        <v>14</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10">
@@ -575,18 +578,15 @@
         <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="K10" s="1">
+        <v>50.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>25</v>
@@ -594,8 +594,11 @@
       <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>31</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12">
@@ -603,33 +606,30 @@
         <v>33</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="K12" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="14">
@@ -643,10 +643,10 @@
         <v>14</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15">
@@ -654,13 +654,30 @@
         <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>39</v>
+      <c r="C16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>